<commit_message>
Audiomoth meta data updated.
</commit_message>
<xml_diff>
--- a/audiomoth_data/audiomoth_metadata.xlsx
+++ b/audiomoth_data/audiomoth_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Documents\University\Year 5 Masters\Research Project\2. Analysis\final_research_project\audiomoth_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7CDF36-D5E5-4F11-A267-1DD49C668FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32A079-5C99-4B1F-B635-11310594030B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="37">
   <si>
     <t>site</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>audiomoth_owner</t>
-  </si>
-  <si>
-    <t>SDcard_ID</t>
   </si>
   <si>
     <t>lat_coord</t>
@@ -116,6 +113,24 @@
   </si>
   <si>
     <t>moorland</t>
+  </si>
+  <si>
+    <t>ashworth</t>
+  </si>
+  <si>
+    <t>SDcard_type</t>
+  </si>
+  <si>
+    <t>SDcard_size</t>
+  </si>
+  <si>
+    <t>SanDiskUltra</t>
+  </si>
+  <si>
+    <t>geosciences</t>
+  </si>
+  <si>
+    <t>SanDiskExtreme</t>
   </si>
 </sst>
 </file>
@@ -477,20 +492,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121:H121"/>
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,2412 +523,3495 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>45792</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>64</v>
+      </c>
+      <c r="H2" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>-3.4026420000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>45793</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>64</v>
+      </c>
+      <c r="H3" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>-3.4026420000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>45794</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>64</v>
+      </c>
+      <c r="H4" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>-3.4026420000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>45792</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>64</v>
+      </c>
+      <c r="H5" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>-3.4047040000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>45793</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="4">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>64</v>
+      </c>
+      <c r="H6" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>-3.4047040000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>45794</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="4">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>64</v>
+      </c>
+      <c r="H7" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>-3.4047040000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>45792</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
+        <v>64</v>
+      </c>
+      <c r="H8" s="4">
         <v>55.776614000000002</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>-3.4009160000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
         <v>45793</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>64</v>
+      </c>
+      <c r="H9" s="4">
         <v>55.776614000000002</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>-3.4009160000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2">
         <v>45794</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <v>64</v>
+      </c>
+      <c r="H10" s="4">
         <v>55.776614000000002</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>-3.4009160000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2">
         <v>45792</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>64</v>
+      </c>
+      <c r="H11" s="4">
         <v>55.775725000000001</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
         <v>45793</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <v>64</v>
+      </c>
+      <c r="H12" s="4">
         <v>55.775725000000001</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>45794</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>64</v>
+      </c>
+      <c r="H13" s="4">
         <v>55.775725000000001</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <v>45792</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="4">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>64</v>
+      </c>
+      <c r="H14" s="4">
         <v>55.776021</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>-3.4005800000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <v>45793</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="4">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15">
+        <v>64</v>
+      </c>
+      <c r="H15" s="4">
         <v>55.776021</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>-3.4005800000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2">
         <v>45794</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="4">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <v>64</v>
+      </c>
+      <c r="H16" s="4">
         <v>55.776021</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="4">
         <v>-3.4005800000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2">
         <v>45792</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="4">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17">
+        <v>64</v>
+      </c>
+      <c r="H17" s="4">
         <v>55.776640999999998</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <v>-3.403073</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2">
         <v>45793</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="4">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18">
+        <v>64</v>
+      </c>
+      <c r="H18" s="4">
         <v>55.776640999999998</v>
       </c>
-      <c r="H18" s="4">
+      <c r="I18" s="4">
         <v>-3.403073</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2">
         <v>45794</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="4">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19">
+        <v>64</v>
+      </c>
+      <c r="H19" s="4">
         <v>55.776640999999998</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <v>-3.403073</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2">
         <v>45792</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="4">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>64</v>
+      </c>
+      <c r="H20" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H20" s="4">
+      <c r="I20" s="4">
         <v>-3.401923</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="2">
         <v>45793</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="4">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21">
+        <v>64</v>
+      </c>
+      <c r="H21" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <v>-3.401923</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2">
         <v>45794</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="4">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22">
+        <v>64</v>
+      </c>
+      <c r="H22" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H22" s="4">
+      <c r="I22" s="4">
         <v>-3.401923</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2">
         <v>45792</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="4">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <v>64</v>
+      </c>
+      <c r="H23" s="4">
         <v>55.776452999999997</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <v>-3.4018269999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2">
         <v>45793</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="4">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24">
+        <v>64</v>
+      </c>
+      <c r="H24" s="4">
         <v>55.776452999999997</v>
       </c>
-      <c r="H24" s="4">
+      <c r="I24" s="4">
         <v>-3.4018269999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2">
         <v>45794</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="4">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25">
+        <v>64</v>
+      </c>
+      <c r="H25" s="4">
         <v>55.776452999999997</v>
       </c>
-      <c r="H25" s="4">
+      <c r="I25" s="4">
         <v>-3.4018269999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2">
         <v>45792</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="4">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26">
+        <v>64</v>
+      </c>
+      <c r="H26" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H26" s="4">
+      <c r="I26" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2">
         <v>45793</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="4">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27">
+        <v>64</v>
+      </c>
+      <c r="H27" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H27" s="4">
+      <c r="I27" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2">
         <v>45794</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="4">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28">
+        <v>64</v>
+      </c>
+      <c r="H28" s="4">
         <v>55.775995000000002</v>
       </c>
-      <c r="H28" s="4">
+      <c r="I28" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="2">
         <v>45792</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="4">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29">
+        <v>64</v>
+      </c>
+      <c r="H29" s="4">
         <v>55.776749000000002</v>
       </c>
-      <c r="H29" s="4">
+      <c r="I29" s="4">
         <v>-3.4024019999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2">
         <v>45793</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="4">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30">
+        <v>64</v>
+      </c>
+      <c r="H30" s="4">
         <v>55.776749000000002</v>
       </c>
-      <c r="H30" s="4">
+      <c r="I30" s="4">
         <v>-3.4024019999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="2">
         <v>45794</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="4">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31">
+        <v>64</v>
+      </c>
+      <c r="H31" s="4">
         <v>55.776749000000002</v>
       </c>
-      <c r="H31" s="4">
+      <c r="I31" s="4">
         <v>-3.4024019999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="2">
         <v>45792</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="4">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32">
+        <v>64</v>
+      </c>
+      <c r="H32" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H32" s="4">
+      <c r="I32" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="2">
         <v>45793</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="4">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33">
+        <v>64</v>
+      </c>
+      <c r="H33" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H33" s="4">
+      <c r="I33" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2">
         <v>45794</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="4">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34">
+        <v>64</v>
+      </c>
+      <c r="H34" s="4">
         <v>55.776209999999999</v>
       </c>
-      <c r="H34" s="4">
+      <c r="I34" s="4">
         <v>-3.4025940000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="2">
         <v>45792</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="4">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35">
+        <v>64</v>
+      </c>
+      <c r="H35" s="4">
         <v>55.776156</v>
       </c>
-      <c r="H35" s="4">
+      <c r="I35" s="4">
         <v>-3.4033129999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="2">
         <v>45793</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="4">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36">
+        <v>64</v>
+      </c>
+      <c r="H36" s="4">
         <v>55.776156</v>
       </c>
-      <c r="H36" s="4">
+      <c r="I36" s="4">
         <v>-3.4033129999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="2">
         <v>45794</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="4">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37">
+        <v>64</v>
+      </c>
+      <c r="H37" s="4">
         <v>55.776156</v>
       </c>
-      <c r="H37" s="4">
+      <c r="I37" s="4">
         <v>-3.4033129999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="2">
         <v>45792</v>
       </c>
       <c r="D38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="4">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38">
+        <v>64</v>
+      </c>
+      <c r="H38" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H38" s="4">
+      <c r="I38" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="2">
         <v>45793</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="4">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39">
+        <v>64</v>
+      </c>
+      <c r="H39" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H39" s="4">
+      <c r="I39" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="2">
         <v>45794</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="4">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40">
+        <v>64</v>
+      </c>
+      <c r="H40" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H40" s="4">
+      <c r="I40" s="4">
         <v>-3.4039839999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="2">
         <v>45792</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="4">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41">
+        <v>64</v>
+      </c>
+      <c r="H41" s="4">
         <v>55.776938000000001</v>
       </c>
-      <c r="H41" s="4">
+      <c r="I41" s="4">
         <v>-3.4015390000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="2">
         <v>45793</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="4">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42">
+        <v>64</v>
+      </c>
+      <c r="H42" s="4">
         <v>55.776938000000001</v>
       </c>
-      <c r="H42" s="4">
+      <c r="I42" s="4">
         <v>-3.4015390000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="2">
         <v>45794</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="4">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43">
+        <v>64</v>
+      </c>
+      <c r="H43" s="4">
         <v>55.776938000000001</v>
       </c>
-      <c r="H43" s="4">
+      <c r="I43" s="4">
         <v>-3.4015390000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" s="2">
         <v>45792</v>
       </c>
       <c r="D44" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="4">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44">
+        <v>64</v>
+      </c>
+      <c r="H44" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H44" s="4">
+      <c r="I44" s="4">
         <v>-3.4033609999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" s="2">
         <v>45793</v>
       </c>
       <c r="D45" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="4">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45">
+        <v>64</v>
+      </c>
+      <c r="H45" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H45" s="4">
+      <c r="I45" s="4">
         <v>-3.4033609999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" s="2">
         <v>45794</v>
       </c>
       <c r="D46" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="4">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" t="s">
+        <v>36</v>
+      </c>
+      <c r="G46">
+        <v>64</v>
+      </c>
+      <c r="H46" s="4">
         <v>55.775886999999997</v>
       </c>
-      <c r="H46" s="4">
+      <c r="I46" s="4">
         <v>-3.4033609999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47" s="2">
         <v>45792</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="4">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47">
+        <v>64</v>
+      </c>
+      <c r="H47" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H47" s="4">
+      <c r="I47" s="4">
         <v>-3.400388</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" s="2">
         <v>45793</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="4">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48">
+        <v>64</v>
+      </c>
+      <c r="H48" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H48" s="4">
+      <c r="I48" s="4">
         <v>-3.400388</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2">
         <v>45794</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="4">
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49">
+        <v>64</v>
+      </c>
+      <c r="H49" s="4">
         <v>55.776398999999998</v>
       </c>
-      <c r="H49" s="4">
+      <c r="I49" s="4">
         <v>-3.400388</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" s="2">
         <v>45792</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" s="4">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50">
+        <v>64</v>
+      </c>
+      <c r="H50" s="4">
         <v>55.776074999999999</v>
       </c>
-      <c r="H50" s="4">
+      <c r="I50" s="4">
         <v>-3.403019</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" s="2">
         <v>45793</v>
       </c>
       <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" s="4">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51">
+        <v>64</v>
+      </c>
+      <c r="H51" s="4">
         <v>55.776074999999999</v>
       </c>
-      <c r="H51" s="4">
+      <c r="I51" s="4">
         <v>-3.403019</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" s="2">
         <v>45794</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
-      </c>
-      <c r="G52" s="4">
+        <v>25</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52">
+        <v>64</v>
+      </c>
+      <c r="H52" s="4">
         <v>55.776074999999999</v>
       </c>
-      <c r="H52" s="4">
+      <c r="I52" s="4">
         <v>-3.403019</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" s="2">
         <v>45792</v>
       </c>
       <c r="D53" t="s">
-        <v>27</v>
-      </c>
-      <c r="G53" s="4">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" t="s">
+        <v>36</v>
+      </c>
+      <c r="G53">
+        <v>64</v>
+      </c>
+      <c r="H53" s="4">
         <v>55.776183000000003</v>
       </c>
-      <c r="H53" s="4">
+      <c r="I53" s="4">
         <v>-3.3997649999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="2">
         <v>45793</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="G54" s="4">
+        <v>26</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G54">
+        <v>64</v>
+      </c>
+      <c r="H54" s="4">
         <v>55.776183000000003</v>
       </c>
-      <c r="H54" s="4">
+      <c r="I54" s="4">
         <v>-3.3997649999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="2">
         <v>45794</v>
       </c>
       <c r="D55" t="s">
-        <v>27</v>
-      </c>
-      <c r="G55" s="4">
+        <v>26</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G55">
+        <v>64</v>
+      </c>
+      <c r="H55" s="4">
         <v>55.776183000000003</v>
       </c>
-      <c r="H55" s="4">
+      <c r="I55" s="4">
         <v>-3.3997649999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C56" s="2">
         <v>45792</v>
       </c>
       <c r="D56" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="4">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G56">
+        <v>64</v>
+      </c>
+      <c r="H56" s="4">
         <v>55.775941000000003</v>
       </c>
-      <c r="H56" s="4">
+      <c r="I56" s="4">
         <v>-3.401443</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57" s="2">
         <v>45793</v>
       </c>
       <c r="D57" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="4">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s">
+        <v>36</v>
+      </c>
+      <c r="G57">
+        <v>64</v>
+      </c>
+      <c r="H57" s="4">
         <v>55.775941000000003</v>
       </c>
-      <c r="H57" s="4">
+      <c r="I57" s="4">
         <v>-3.401443</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="2">
         <v>45794</v>
       </c>
       <c r="D58" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="4">
+        <v>27</v>
+      </c>
+      <c r="E58" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58">
+        <v>64</v>
+      </c>
+      <c r="H58" s="4">
         <v>55.775941000000003</v>
       </c>
-      <c r="H58" s="4">
+      <c r="I58" s="4">
         <v>-3.401443</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59" s="2">
         <v>45792</v>
       </c>
       <c r="D59" t="s">
-        <v>29</v>
-      </c>
-      <c r="G59" s="4">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59">
+        <v>64</v>
+      </c>
+      <c r="H59" s="4">
         <v>55.776291000000001</v>
       </c>
-      <c r="H59" s="4">
+      <c r="I59" s="4">
         <v>-3.4011559999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60" s="2">
         <v>45793</v>
       </c>
       <c r="D60" t="s">
-        <v>29</v>
-      </c>
-      <c r="G60" s="4">
+        <v>28</v>
+      </c>
+      <c r="E60" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60">
+        <v>64</v>
+      </c>
+      <c r="H60" s="4">
         <v>55.776291000000001</v>
       </c>
-      <c r="H60" s="4">
+      <c r="I60" s="4">
         <v>-3.4011559999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61" s="2">
         <v>45794</v>
       </c>
       <c r="D61" t="s">
-        <v>29</v>
-      </c>
-      <c r="G61" s="4">
+        <v>28</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="s">
+        <v>36</v>
+      </c>
+      <c r="G61">
+        <v>64</v>
+      </c>
+      <c r="H61" s="4">
         <v>55.776291000000001</v>
       </c>
-      <c r="H61" s="4">
+      <c r="I61" s="4">
         <v>-3.4011559999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" s="2">
         <v>45798</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="4">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" t="s">
+        <v>36</v>
+      </c>
+      <c r="G62">
+        <v>64</v>
+      </c>
+      <c r="H62" s="4">
         <v>55.781802399999997</v>
       </c>
-      <c r="H62" s="4">
+      <c r="I62" s="4">
         <v>-3.4046675999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C63" s="2">
         <v>45799</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="4">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" t="s">
+        <v>36</v>
+      </c>
+      <c r="G63">
+        <v>64</v>
+      </c>
+      <c r="H63" s="4">
         <v>55.781802399999997</v>
       </c>
-      <c r="H63" s="4">
+      <c r="I63" s="4">
         <v>-3.4046675999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" s="2">
         <v>45800</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="4">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" t="s">
+        <v>36</v>
+      </c>
+      <c r="G64">
+        <v>64</v>
+      </c>
+      <c r="H64" s="4">
         <v>55.781802399999997</v>
       </c>
-      <c r="H64" s="4">
+      <c r="I64" s="4">
         <v>-3.4046675999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65" s="2">
         <v>45798</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" s="4">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65">
+        <v>64</v>
+      </c>
+      <c r="H65" s="4">
         <v>55.7830327</v>
       </c>
-      <c r="H65" s="4">
+      <c r="I65" s="4">
         <v>-3.4032567999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C66" s="2">
         <v>45799</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
-      </c>
-      <c r="G66" s="4">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>31</v>
+      </c>
+      <c r="F66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66">
+        <v>64</v>
+      </c>
+      <c r="H66" s="4">
         <v>55.7830327</v>
       </c>
-      <c r="H66" s="4">
+      <c r="I66" s="4">
         <v>-3.4032567999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C67" s="2">
         <v>45800</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="4">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67">
+        <v>64</v>
+      </c>
+      <c r="H67" s="4">
         <v>55.7830327</v>
       </c>
-      <c r="H67" s="4">
+      <c r="I67" s="4">
         <v>-3.4032567999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C68" s="2">
         <v>45798</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="4">
+        <v>11</v>
+      </c>
+      <c r="E68" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68">
+        <v>64</v>
+      </c>
+      <c r="H68" s="4">
         <v>55.782387900000003</v>
       </c>
-      <c r="H68" s="4">
+      <c r="I68" s="4">
         <v>-3.4023837000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C69" s="2">
         <v>45799</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="4">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>35</v>
+      </c>
+      <c r="F69" t="s">
+        <v>36</v>
+      </c>
+      <c r="G69">
+        <v>64</v>
+      </c>
+      <c r="H69" s="4">
         <v>55.782387900000003</v>
       </c>
-      <c r="H69" s="4">
+      <c r="I69" s="4">
         <v>-3.4023837000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" s="2">
         <v>45800</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="4">
+        <v>11</v>
+      </c>
+      <c r="E70" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" t="s">
+        <v>36</v>
+      </c>
+      <c r="G70">
+        <v>64</v>
+      </c>
+      <c r="H70" s="4">
         <v>55.782387900000003</v>
       </c>
-      <c r="H70" s="4">
+      <c r="I70" s="4">
         <v>-3.4023837000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C71" s="2">
         <v>45798</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
-      </c>
-      <c r="G71" s="4">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>31</v>
+      </c>
+      <c r="F71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71">
+        <v>64</v>
+      </c>
+      <c r="H71" s="4">
         <v>55.781562399999999</v>
       </c>
-      <c r="H71" s="4">
+      <c r="I71" s="4">
         <v>-3.4053393999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" s="2">
         <v>45799</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" s="4">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>31</v>
+      </c>
+      <c r="F72" t="s">
+        <v>34</v>
+      </c>
+      <c r="G72">
+        <v>64</v>
+      </c>
+      <c r="H72" s="4">
         <v>55.781562399999999</v>
       </c>
-      <c r="H72" s="4">
+      <c r="I72" s="4">
         <v>-3.4053393999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" s="2">
         <v>45800</v>
       </c>
       <c r="D73" t="s">
-        <v>13</v>
-      </c>
-      <c r="G73" s="4">
+        <v>12</v>
+      </c>
+      <c r="E73" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73">
+        <v>64</v>
+      </c>
+      <c r="H73" s="4">
         <v>55.781562399999999</v>
       </c>
-      <c r="H73" s="4">
+      <c r="I73" s="4">
         <v>-3.4053393999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C74" s="2">
         <v>45798</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" s="4">
+        <v>13</v>
+      </c>
+      <c r="E74" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74">
+        <v>64</v>
+      </c>
+      <c r="H74" s="4">
         <v>55.781238000000002</v>
       </c>
-      <c r="H74" s="4">
+      <c r="I74" s="4">
         <v>-3.4048367000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C75" s="2">
         <v>45799</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" s="4">
+        <v>13</v>
+      </c>
+      <c r="E75" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" t="s">
+        <v>36</v>
+      </c>
+      <c r="G75">
+        <v>64</v>
+      </c>
+      <c r="H75" s="4">
         <v>55.781238000000002</v>
       </c>
-      <c r="H75" s="4">
+      <c r="I75" s="4">
         <v>-3.4048367000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C76" s="2">
         <v>45800</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
-      </c>
-      <c r="G76" s="4">
+        <v>13</v>
+      </c>
+      <c r="E76" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" t="s">
+        <v>36</v>
+      </c>
+      <c r="G76">
+        <v>64</v>
+      </c>
+      <c r="H76" s="4">
         <v>55.781238000000002</v>
       </c>
-      <c r="H76" s="4">
+      <c r="I76" s="4">
         <v>-3.4048367000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C77" s="2">
         <v>45798</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G77" s="4">
+        <v>14</v>
+      </c>
+      <c r="E77" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" t="s">
+        <v>36</v>
+      </c>
+      <c r="G77">
+        <v>64</v>
+      </c>
+      <c r="H77" s="4">
         <v>55.782174500000004</v>
       </c>
-      <c r="H77" s="4">
+      <c r="I77" s="4">
         <v>-3.4052387</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C78" s="2">
         <v>45799</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="4">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" t="s">
+        <v>36</v>
+      </c>
+      <c r="G78">
+        <v>64</v>
+      </c>
+      <c r="H78" s="4">
         <v>55.782174500000004</v>
       </c>
-      <c r="H78" s="4">
+      <c r="I78" s="4">
         <v>-3.4052387</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C79" s="2">
         <v>45800</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
-      </c>
-      <c r="G79" s="4">
+        <v>14</v>
+      </c>
+      <c r="E79" t="s">
+        <v>35</v>
+      </c>
+      <c r="F79" t="s">
+        <v>36</v>
+      </c>
+      <c r="G79">
+        <v>64</v>
+      </c>
+      <c r="H79" s="4">
         <v>55.782174500000004</v>
       </c>
-      <c r="H79" s="4">
+      <c r="I79" s="4">
         <v>-3.4052387</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C80" s="2">
         <v>45798</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="4">
+        <v>15</v>
+      </c>
+      <c r="E80" t="s">
+        <v>35</v>
+      </c>
+      <c r="F80" t="s">
+        <v>36</v>
+      </c>
+      <c r="G80">
+        <v>64</v>
+      </c>
+      <c r="H80" s="4">
         <v>55.783175399999998</v>
       </c>
-      <c r="H80" s="4">
+      <c r="I80" s="4">
         <v>-3.4047087</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C81" s="2">
         <v>45799</v>
       </c>
       <c r="D81" t="s">
-        <v>16</v>
-      </c>
-      <c r="G81" s="4">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
+        <v>35</v>
+      </c>
+      <c r="F81" t="s">
+        <v>36</v>
+      </c>
+      <c r="G81">
+        <v>64</v>
+      </c>
+      <c r="H81" s="4">
         <v>55.783175399999998</v>
       </c>
-      <c r="H81" s="4">
+      <c r="I81" s="4">
         <v>-3.4047087</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C82" s="2">
         <v>45800</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" s="4">
+        <v>15</v>
+      </c>
+      <c r="E82" t="s">
+        <v>35</v>
+      </c>
+      <c r="F82" t="s">
+        <v>36</v>
+      </c>
+      <c r="G82">
+        <v>64</v>
+      </c>
+      <c r="H82" s="4">
         <v>55.783175399999998</v>
       </c>
-      <c r="H82" s="4">
+      <c r="I82" s="4">
         <v>-3.4047087</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" s="2">
         <v>45798</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
-      </c>
-      <c r="G83" s="4">
+        <v>16</v>
+      </c>
+      <c r="E83" t="s">
+        <v>35</v>
+      </c>
+      <c r="F83" t="s">
+        <v>36</v>
+      </c>
+      <c r="G83">
+        <v>64</v>
+      </c>
+      <c r="H83" s="4">
         <v>55.7821012</v>
       </c>
-      <c r="H83" s="4">
+      <c r="I83" s="4">
         <v>-3.4029975000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C84" s="2">
         <v>45799</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
-      </c>
-      <c r="G84" s="4">
+        <v>16</v>
+      </c>
+      <c r="E84" t="s">
+        <v>35</v>
+      </c>
+      <c r="F84" t="s">
+        <v>36</v>
+      </c>
+      <c r="G84">
+        <v>64</v>
+      </c>
+      <c r="H84" s="4">
         <v>55.7821012</v>
       </c>
-      <c r="H84" s="4">
+      <c r="I84" s="4">
         <v>-3.4029975000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C85" s="2">
         <v>45800</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
-      </c>
-      <c r="G85" s="4">
+        <v>16</v>
+      </c>
+      <c r="E85" t="s">
+        <v>35</v>
+      </c>
+      <c r="F85" t="s">
+        <v>36</v>
+      </c>
+      <c r="G85">
+        <v>64</v>
+      </c>
+      <c r="H85" s="4">
         <v>55.7821012</v>
       </c>
-      <c r="H85" s="4">
+      <c r="I85" s="4">
         <v>-3.4029975000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C86" s="2">
         <v>45798</v>
       </c>
       <c r="D86" t="s">
-        <v>18</v>
-      </c>
-      <c r="G86" s="4">
+        <v>17</v>
+      </c>
+      <c r="E86" t="s">
+        <v>31</v>
+      </c>
+      <c r="F86" t="s">
+        <v>36</v>
+      </c>
+      <c r="G86">
+        <v>64</v>
+      </c>
+      <c r="H86" s="4">
         <v>55.782734599999998</v>
       </c>
-      <c r="H86" s="4">
+      <c r="I86" s="4">
         <v>-3.4028046000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C87" s="2">
         <v>45799</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
-      </c>
-      <c r="G87" s="4">
+        <v>17</v>
+      </c>
+      <c r="E87" t="s">
+        <v>31</v>
+      </c>
+      <c r="F87" t="s">
+        <v>36</v>
+      </c>
+      <c r="G87">
+        <v>64</v>
+      </c>
+      <c r="H87" s="4">
         <v>55.782734599999998</v>
       </c>
-      <c r="H87" s="4">
+      <c r="I87" s="4">
         <v>-3.4028046000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C88" s="2">
         <v>45800</v>
       </c>
       <c r="D88" t="s">
-        <v>18</v>
-      </c>
-      <c r="G88" s="4">
+        <v>17</v>
+      </c>
+      <c r="E88" t="s">
+        <v>31</v>
+      </c>
+      <c r="F88" t="s">
+        <v>36</v>
+      </c>
+      <c r="G88">
+        <v>64</v>
+      </c>
+      <c r="H88" s="4">
         <v>55.782734599999998</v>
       </c>
-      <c r="H88" s="4">
+      <c r="I88" s="4">
         <v>-3.4028046000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C89" s="2">
         <v>45798</v>
       </c>
       <c r="D89" t="s">
-        <v>19</v>
-      </c>
-      <c r="G89" s="4">
+        <v>18</v>
+      </c>
+      <c r="E89" t="s">
+        <v>31</v>
+      </c>
+      <c r="F89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89">
+        <v>64</v>
+      </c>
+      <c r="H89" s="4">
         <v>55.782073099999998</v>
       </c>
-      <c r="H89" s="4">
+      <c r="I89" s="4">
         <v>-3.4041242999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C90" s="2">
         <v>45799</v>
       </c>
       <c r="D90" t="s">
-        <v>19</v>
-      </c>
-      <c r="G90" s="4">
+        <v>18</v>
+      </c>
+      <c r="E90" t="s">
+        <v>31</v>
+      </c>
+      <c r="F90" t="s">
+        <v>34</v>
+      </c>
+      <c r="G90">
+        <v>64</v>
+      </c>
+      <c r="H90" s="4">
         <v>55.782073099999998</v>
       </c>
-      <c r="H90" s="4">
+      <c r="I90" s="4">
         <v>-3.4041242999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C91" s="2">
         <v>45800</v>
       </c>
       <c r="D91" t="s">
-        <v>19</v>
-      </c>
-      <c r="G91" s="4">
+        <v>18</v>
+      </c>
+      <c r="E91" t="s">
+        <v>31</v>
+      </c>
+      <c r="F91" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91">
+        <v>64</v>
+      </c>
+      <c r="H91" s="4">
         <v>55.782073099999998</v>
       </c>
-      <c r="H91" s="4">
+      <c r="I91" s="4">
         <v>-3.4041242999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C92" s="2">
         <v>45798</v>
       </c>
       <c r="D92" t="s">
-        <v>20</v>
-      </c>
-      <c r="G92" s="4">
+        <v>19</v>
+      </c>
+      <c r="E92" t="s">
+        <v>35</v>
+      </c>
+      <c r="F92" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92">
+        <v>64</v>
+      </c>
+      <c r="H92" s="4">
         <v>55.7825512</v>
       </c>
-      <c r="H92" s="4">
+      <c r="I92" s="4">
         <v>-3.4057582000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C93" s="2">
         <v>45799</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
-      </c>
-      <c r="G93" s="4">
+        <v>19</v>
+      </c>
+      <c r="E93" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93" t="s">
+        <v>36</v>
+      </c>
+      <c r="G93">
+        <v>64</v>
+      </c>
+      <c r="H93" s="4">
         <v>55.7825512</v>
       </c>
-      <c r="H93" s="4">
+      <c r="I93" s="4">
         <v>-3.4057582000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" s="2">
         <v>45800</v>
       </c>
       <c r="D94" t="s">
-        <v>20</v>
-      </c>
-      <c r="G94" s="4">
+        <v>19</v>
+      </c>
+      <c r="E94" t="s">
+        <v>35</v>
+      </c>
+      <c r="F94" t="s">
+        <v>36</v>
+      </c>
+      <c r="G94">
+        <v>64</v>
+      </c>
+      <c r="H94" s="4">
         <v>55.7825512</v>
       </c>
-      <c r="H94" s="4">
+      <c r="I94" s="4">
         <v>-3.4057582000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C95" s="2">
         <v>45798</v>
       </c>
       <c r="D95" t="s">
-        <v>21</v>
-      </c>
-      <c r="G95" s="4">
+        <v>20</v>
+      </c>
+      <c r="E95" t="s">
+        <v>35</v>
+      </c>
+      <c r="F95" t="s">
+        <v>36</v>
+      </c>
+      <c r="G95">
+        <v>64</v>
+      </c>
+      <c r="H95" s="4">
         <v>55.782199900000002</v>
       </c>
-      <c r="H95" s="4">
+      <c r="I95" s="4">
         <v>-3.4063479999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C96" s="2">
         <v>45799</v>
       </c>
       <c r="D96" t="s">
-        <v>21</v>
-      </c>
-      <c r="G96" s="4">
+        <v>20</v>
+      </c>
+      <c r="E96" t="s">
+        <v>35</v>
+      </c>
+      <c r="F96" t="s">
+        <v>36</v>
+      </c>
+      <c r="G96">
+        <v>64</v>
+      </c>
+      <c r="H96" s="4">
         <v>55.782199900000002</v>
       </c>
-      <c r="H96" s="4">
+      <c r="I96" s="4">
         <v>-3.4063479999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97" s="2">
         <v>45800</v>
       </c>
       <c r="D97" t="s">
-        <v>21</v>
-      </c>
-      <c r="G97" s="4">
+        <v>20</v>
+      </c>
+      <c r="E97" t="s">
+        <v>35</v>
+      </c>
+      <c r="F97" t="s">
+        <v>36</v>
+      </c>
+      <c r="G97">
+        <v>64</v>
+      </c>
+      <c r="H97" s="4">
         <v>55.782199900000002</v>
       </c>
-      <c r="H97" s="4">
+      <c r="I97" s="4">
         <v>-3.4063479999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C98" s="2">
         <v>45798</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
-      </c>
-      <c r="G98" s="4">
+        <v>21</v>
+      </c>
+      <c r="E98" t="s">
+        <v>35</v>
+      </c>
+      <c r="F98" t="s">
+        <v>36</v>
+      </c>
+      <c r="G98">
+        <v>64</v>
+      </c>
+      <c r="H98" s="4">
         <v>55.782838400000003</v>
       </c>
-      <c r="H98" s="4">
+      <c r="I98" s="4">
         <v>-3.4052527000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C99" s="2">
         <v>45799</v>
       </c>
       <c r="D99" t="s">
-        <v>22</v>
-      </c>
-      <c r="G99" s="4">
+        <v>21</v>
+      </c>
+      <c r="E99" t="s">
+        <v>35</v>
+      </c>
+      <c r="F99" t="s">
+        <v>36</v>
+      </c>
+      <c r="G99">
+        <v>64</v>
+      </c>
+      <c r="H99" s="4">
         <v>55.782838400000003</v>
       </c>
-      <c r="H99" s="4">
+      <c r="I99" s="4">
         <v>-3.4052527000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B100" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C100" s="2">
         <v>45800</v>
       </c>
       <c r="D100" t="s">
-        <v>22</v>
-      </c>
-      <c r="G100" s="4">
+        <v>21</v>
+      </c>
+      <c r="E100" t="s">
+        <v>35</v>
+      </c>
+      <c r="F100" t="s">
+        <v>36</v>
+      </c>
+      <c r="G100">
+        <v>64</v>
+      </c>
+      <c r="H100" s="4">
         <v>55.782838400000003</v>
       </c>
-      <c r="H100" s="4">
+      <c r="I100" s="4">
         <v>-3.4052527000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C101" s="2">
         <v>45798</v>
       </c>
       <c r="D101" t="s">
-        <v>23</v>
-      </c>
-      <c r="G101" s="4">
+        <v>22</v>
+      </c>
+      <c r="E101" t="s">
+        <v>35</v>
+      </c>
+      <c r="F101" t="s">
+        <v>36</v>
+      </c>
+      <c r="G101">
+        <v>64</v>
+      </c>
+      <c r="H101" s="4">
         <v>55.7828327</v>
       </c>
-      <c r="H101" s="4">
+      <c r="I101" s="4">
         <v>-3.4041681000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B102" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C102" s="2">
         <v>45799</v>
       </c>
       <c r="D102" t="s">
-        <v>23</v>
-      </c>
-      <c r="G102" s="4">
+        <v>22</v>
+      </c>
+      <c r="E102" t="s">
+        <v>35</v>
+      </c>
+      <c r="F102" t="s">
+        <v>36</v>
+      </c>
+      <c r="G102">
+        <v>64</v>
+      </c>
+      <c r="H102" s="4">
         <v>55.7828327</v>
       </c>
-      <c r="H102" s="4">
+      <c r="I102" s="4">
         <v>-3.4041681000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C103" s="2">
         <v>45800</v>
       </c>
       <c r="D103" t="s">
-        <v>23</v>
-      </c>
-      <c r="G103" s="4">
+        <v>22</v>
+      </c>
+      <c r="E103" t="s">
+        <v>35</v>
+      </c>
+      <c r="F103" t="s">
+        <v>36</v>
+      </c>
+      <c r="G103">
+        <v>64</v>
+      </c>
+      <c r="H103" s="4">
         <v>55.7828327</v>
       </c>
-      <c r="H103" s="4">
+      <c r="I103" s="4">
         <v>-3.4041681000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B104" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C104" s="2">
         <v>45798</v>
       </c>
       <c r="D104" t="s">
-        <v>24</v>
-      </c>
-      <c r="G104" s="4">
+        <v>23</v>
+      </c>
+      <c r="E104" t="s">
+        <v>35</v>
+      </c>
+      <c r="F104" t="s">
+        <v>36</v>
+      </c>
+      <c r="G104">
+        <v>64</v>
+      </c>
+      <c r="H104" s="4">
         <v>55.782456500000002</v>
       </c>
-      <c r="H104" s="4">
+      <c r="I104" s="4">
         <v>-3.4036138</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C105" s="2">
         <v>45799</v>
       </c>
       <c r="D105" t="s">
-        <v>24</v>
-      </c>
-      <c r="G105" s="4">
+        <v>23</v>
+      </c>
+      <c r="E105" t="s">
+        <v>35</v>
+      </c>
+      <c r="F105" t="s">
+        <v>36</v>
+      </c>
+      <c r="G105">
+        <v>64</v>
+      </c>
+      <c r="H105" s="4">
         <v>55.782456500000002</v>
       </c>
-      <c r="H105" s="4">
+      <c r="I105" s="4">
         <v>-3.4036138</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C106" s="2">
         <v>45800</v>
       </c>
       <c r="D106" t="s">
-        <v>24</v>
-      </c>
-      <c r="G106" s="4">
+        <v>23</v>
+      </c>
+      <c r="E106" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" t="s">
+        <v>36</v>
+      </c>
+      <c r="G106">
+        <v>64</v>
+      </c>
+      <c r="H106" s="4">
         <v>55.782456500000002</v>
       </c>
-      <c r="H106" s="4">
+      <c r="I106" s="4">
         <v>-3.4036138</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C107" s="2">
         <v>45798</v>
       </c>
       <c r="D107" t="s">
-        <v>25</v>
-      </c>
-      <c r="G107" s="4">
+        <v>24</v>
+      </c>
+      <c r="E107" t="s">
+        <v>35</v>
+      </c>
+      <c r="F107" t="s">
+        <v>36</v>
+      </c>
+      <c r="G107">
+        <v>64</v>
+      </c>
+      <c r="H107" s="4">
         <v>55.781897600000001</v>
       </c>
-      <c r="H107" s="4">
+      <c r="I107" s="4">
         <v>-3.4058609</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C108" s="2">
         <v>45799</v>
       </c>
       <c r="D108" t="s">
-        <v>25</v>
-      </c>
-      <c r="G108" s="4">
+        <v>24</v>
+      </c>
+      <c r="E108" t="s">
+        <v>35</v>
+      </c>
+      <c r="F108" t="s">
+        <v>36</v>
+      </c>
+      <c r="G108">
+        <v>64</v>
+      </c>
+      <c r="H108" s="4">
         <v>55.781897600000001</v>
       </c>
-      <c r="H108" s="4">
+      <c r="I108" s="4">
         <v>-3.4058609</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C109" s="2">
         <v>45800</v>
       </c>
       <c r="D109" t="s">
-        <v>25</v>
-      </c>
-      <c r="G109" s="4">
+        <v>24</v>
+      </c>
+      <c r="E109" t="s">
+        <v>35</v>
+      </c>
+      <c r="F109" t="s">
+        <v>36</v>
+      </c>
+      <c r="G109">
+        <v>64</v>
+      </c>
+      <c r="H109" s="4">
         <v>55.781897600000001</v>
       </c>
-      <c r="H109" s="4">
+      <c r="I109" s="4">
         <v>-3.4058609</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C110" s="2">
         <v>45798</v>
       </c>
       <c r="D110" t="s">
-        <v>26</v>
-      </c>
-      <c r="G110" s="4">
+        <v>25</v>
+      </c>
+      <c r="E110" t="s">
+        <v>35</v>
+      </c>
+      <c r="F110" t="s">
+        <v>36</v>
+      </c>
+      <c r="G110">
+        <v>64</v>
+      </c>
+      <c r="H110" s="4">
         <v>55.7818045</v>
       </c>
-      <c r="H110" s="4">
+      <c r="I110" s="4">
         <v>-3.4036038</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C111" s="2">
         <v>45799</v>
       </c>
       <c r="D111" t="s">
-        <v>26</v>
-      </c>
-      <c r="G111" s="4">
+        <v>25</v>
+      </c>
+      <c r="E111" t="s">
+        <v>35</v>
+      </c>
+      <c r="F111" t="s">
+        <v>36</v>
+      </c>
+      <c r="G111">
+        <v>64</v>
+      </c>
+      <c r="H111" s="4">
         <v>55.7818045</v>
       </c>
-      <c r="H111" s="4">
+      <c r="I111" s="4">
         <v>-3.4036038</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C112" s="2">
         <v>45800</v>
       </c>
       <c r="D112" t="s">
-        <v>26</v>
-      </c>
-      <c r="G112" s="4">
+        <v>25</v>
+      </c>
+      <c r="E112" t="s">
+        <v>35</v>
+      </c>
+      <c r="F112" t="s">
+        <v>36</v>
+      </c>
+      <c r="G112">
+        <v>64</v>
+      </c>
+      <c r="H112" s="4">
         <v>55.7818045</v>
       </c>
-      <c r="H112" s="4">
+      <c r="I112" s="4">
         <v>-3.4036038</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C113" s="2">
         <v>45798</v>
       </c>
       <c r="D113" t="s">
-        <v>27</v>
-      </c>
-      <c r="G113" s="4">
+        <v>26</v>
+      </c>
+      <c r="E113" t="s">
+        <v>35</v>
+      </c>
+      <c r="F113" t="s">
+        <v>36</v>
+      </c>
+      <c r="G113">
+        <v>64</v>
+      </c>
+      <c r="H113" s="4">
         <v>55.782467500000003</v>
       </c>
-      <c r="H113" s="4">
+      <c r="I113" s="4">
         <v>-3.4046557000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C114" s="2">
         <v>45799</v>
       </c>
       <c r="D114" t="s">
-        <v>27</v>
-      </c>
-      <c r="G114" s="4">
+        <v>26</v>
+      </c>
+      <c r="E114" t="s">
+        <v>35</v>
+      </c>
+      <c r="F114" t="s">
+        <v>36</v>
+      </c>
+      <c r="G114">
+        <v>64</v>
+      </c>
+      <c r="H114" s="4">
         <v>55.782467500000003</v>
       </c>
-      <c r="H114" s="4">
+      <c r="I114" s="4">
         <v>-3.4046557000000002</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C115" s="2">
         <v>45800</v>
       </c>
       <c r="D115" t="s">
-        <v>27</v>
-      </c>
-      <c r="G115" s="4">
+        <v>26</v>
+      </c>
+      <c r="E115" t="s">
+        <v>35</v>
+      </c>
+      <c r="F115" t="s">
+        <v>36</v>
+      </c>
+      <c r="G115">
+        <v>64</v>
+      </c>
+      <c r="H115" s="4">
         <v>55.782467500000003</v>
       </c>
-      <c r="H115" s="4">
+      <c r="I115" s="4">
         <v>-3.4046557000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C116" s="2">
         <v>45798</v>
       </c>
       <c r="D116" t="s">
-        <v>28</v>
-      </c>
-      <c r="G116" s="4">
+        <v>27</v>
+      </c>
+      <c r="E116" t="s">
+        <v>35</v>
+      </c>
+      <c r="F116" t="s">
+        <v>36</v>
+      </c>
+      <c r="G116">
+        <v>64</v>
+      </c>
+      <c r="H116" s="4">
         <v>55.783361900000003</v>
       </c>
-      <c r="H116" s="4">
+      <c r="I116" s="4">
         <v>-3.4037117000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C117" s="2">
         <v>45799</v>
       </c>
       <c r="D117" t="s">
-        <v>28</v>
-      </c>
-      <c r="G117" s="4">
+        <v>27</v>
+      </c>
+      <c r="E117" t="s">
+        <v>35</v>
+      </c>
+      <c r="F117" t="s">
+        <v>36</v>
+      </c>
+      <c r="G117">
+        <v>64</v>
+      </c>
+      <c r="H117" s="4">
         <v>55.783361900000003</v>
       </c>
-      <c r="H117" s="4">
+      <c r="I117" s="4">
         <v>-3.4037117000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C118" s="2">
         <v>45800</v>
       </c>
       <c r="D118" t="s">
-        <v>28</v>
-      </c>
-      <c r="G118" s="4">
+        <v>27</v>
+      </c>
+      <c r="E118" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" t="s">
+        <v>36</v>
+      </c>
+      <c r="G118">
+        <v>64</v>
+      </c>
+      <c r="H118" s="4">
         <v>55.783361900000003</v>
       </c>
-      <c r="H118" s="4">
+      <c r="I118" s="4">
         <v>-3.4037117000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C119" s="2">
         <v>45798</v>
       </c>
       <c r="D119" t="s">
-        <v>29</v>
-      </c>
-      <c r="G119" s="4">
+        <v>28</v>
+      </c>
+      <c r="E119" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" t="s">
+        <v>36</v>
+      </c>
+      <c r="G119">
+        <v>64</v>
+      </c>
+      <c r="H119" s="4">
         <v>55.781531999999999</v>
       </c>
-      <c r="H119" s="4">
+      <c r="I119" s="4">
         <v>-3.4041983999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B120" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C120" s="2">
         <v>45799</v>
       </c>
       <c r="D120" t="s">
-        <v>29</v>
-      </c>
-      <c r="G120" s="4">
+        <v>28</v>
+      </c>
+      <c r="E120" t="s">
+        <v>35</v>
+      </c>
+      <c r="F120" t="s">
+        <v>36</v>
+      </c>
+      <c r="G120">
+        <v>64</v>
+      </c>
+      <c r="H120" s="4">
         <v>55.781531999999999</v>
       </c>
-      <c r="H120" s="4">
+      <c r="I120" s="4">
         <v>-3.4041983999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B121" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C121" s="2">
         <v>45800</v>
       </c>
       <c r="D121" t="s">
-        <v>29</v>
-      </c>
-      <c r="G121" s="4">
+        <v>28</v>
+      </c>
+      <c r="E121" t="s">
+        <v>35</v>
+      </c>
+      <c r="F121" t="s">
+        <v>36</v>
+      </c>
+      <c r="G121">
+        <v>64</v>
+      </c>
+      <c r="H121" s="4">
         <v>55.781531999999999</v>
       </c>
-      <c r="H121" s="4">
+      <c r="I121" s="4">
         <v>-3.4041983999999998</v>
       </c>
     </row>

</xml_diff>